<commit_message>
Fixed issue where site would not record
</commit_message>
<xml_diff>
--- a/Output/Example.xlsx
+++ b/Output/Example.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2174" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2177" uniqueCount="149">
   <si>
     <t>Match ID</t>
   </si>
@@ -225,163 +225,163 @@
     <t>Asylum</t>
   </si>
   <si>
-    <t>Iana</t>
+    <t>iana</t>
   </si>
   <si>
-    <t>Hibana</t>
+    <t>hibana</t>
   </si>
   <si>
-    <t>Sledge</t>
+    <t>sledge</t>
   </si>
   <si>
-    <t>Grim</t>
+    <t>grim</t>
   </si>
   <si>
-    <t>Ying</t>
+    <t>ying</t>
   </si>
   <si>
-    <t>Ace</t>
+    <t>ace</t>
   </si>
   <si>
-    <t>Thatcher</t>
+    <t>thatcher</t>
   </si>
   <si>
-    <t>Maverick</t>
+    <t>maverick</t>
   </si>
   <si>
-    <t>Ash</t>
+    <t>ash</t>
   </si>
   <si>
-    <t>Capitao</t>
+    <t>capitao</t>
   </si>
   <si>
-    <t>Amaru</t>
+    <t>amaru</t>
   </si>
   <si>
-    <t>Jager</t>
+    <t>jäger</t>
   </si>
   <si>
-    <t>Azami</t>
+    <t>azami</t>
   </si>
   <si>
-    <t>Fenrir</t>
+    <t>fenrir</t>
   </si>
   <si>
-    <t>Tachanka</t>
+    <t>tachanka</t>
   </si>
   <si>
-    <t>Solis</t>
+    <t>solis</t>
   </si>
   <si>
-    <t>Wamai</t>
+    <t>wamai</t>
   </si>
   <si>
-    <t>Mute</t>
+    <t>mute</t>
   </si>
   <si>
-    <t>Castle</t>
+    <t>castle</t>
   </si>
   <si>
-    <t>Kaid</t>
+    <t>kaid</t>
   </si>
   <si>
-    <t>Frost</t>
+    <t>frost</t>
   </si>
   <si>
-    <t>Warden</t>
+    <t>warden</t>
   </si>
   <si>
-    <t>Kapkan</t>
+    <t>kapkan</t>
   </si>
   <si>
-    <t>Pulse</t>
+    <t>pulse</t>
   </si>
   <si>
-    <t>Mozzie</t>
+    <t>mozzie</t>
   </si>
   <si>
-    <t>Mira</t>
+    <t>mira</t>
   </si>
   <si>
-    <t>Aruni</t>
+    <t>aruni</t>
   </si>
   <si>
-    <t>Buck</t>
+    <t>buck</t>
   </si>
   <si>
-    <t>Nomad</t>
+    <t>nomad</t>
   </si>
   <si>
-    <t>Jackal</t>
+    <t>jackal</t>
   </si>
   <si>
-    <t>Zofia</t>
+    <t>zofia</t>
   </si>
   <si>
-    <t>Lion</t>
+    <t>lion</t>
   </si>
   <si>
-    <t>IQ</t>
+    <t>iq</t>
   </si>
   <si>
-    <t>Dokkaebi</t>
+    <t>dokkaebi</t>
   </si>
   <si>
-    <t>Blitz</t>
+    <t>blitz</t>
   </si>
   <si>
-    <t>Bandit</t>
+    <t>bandit</t>
   </si>
   <si>
-    <t>Doc</t>
+    <t>doc</t>
   </si>
   <si>
-    <t>Finka</t>
+    <t>finka</t>
   </si>
   <si>
-    <t>Thermite</t>
+    <t>thermite</t>
   </si>
   <si>
-    <t>Osa</t>
+    <t>osa</t>
   </si>
   <si>
-    <t>Twitch</t>
+    <t>twitch</t>
   </si>
   <si>
-    <t>Vigil</t>
+    <t>vigil</t>
   </si>
   <si>
-    <t>Goyo</t>
+    <t>goyo</t>
   </si>
   <si>
-    <t>Smoke</t>
+    <t>smoke</t>
   </si>
   <si>
-    <t>Maestro</t>
+    <t>maestro</t>
   </si>
   <si>
-    <t>Oryx</t>
+    <t>oryx</t>
   </si>
   <si>
-    <t>Brava</t>
+    <t>brava</t>
   </si>
   <si>
-    <t>Nokk</t>
+    <t>nokk</t>
   </si>
   <si>
-    <t>Gridlock</t>
+    <t>gridlock</t>
   </si>
   <si>
-    <t>Echo</t>
+    <t>echo</t>
   </si>
   <si>
-    <t>Valkyrie</t>
+    <t>valkyrie</t>
   </si>
   <si>
-    <t>Alibi</t>
+    <t>alibi</t>
   </si>
   <si>
-    <t>Fuze</t>
+    <t>fuze</t>
   </si>
   <si>
     <t>Junkyard</t>
@@ -1039,6 +1039,9 @@
       <c r="C8" t="s">
         <v>20</v>
       </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
       <c r="E8" t="s">
         <v>44</v>
       </c>
@@ -1065,6 +1068,9 @@
       <c r="C9" t="s">
         <v>20</v>
       </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
       <c r="E9" t="s">
         <v>44</v>
       </c>
@@ -1091,6 +1097,9 @@
       <c r="C10" t="s">
         <v>20</v>
       </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
       <c r="E10" t="s">
         <v>44</v>
       </c>
@@ -3209,7 +3218,7 @@
         <v>42</v>
       </c>
       <c r="E83" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F83" t="b">
         <v>0</v>
@@ -4708,7 +4717,7 @@
         <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>122</v>
+        <v>26</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -4755,7 +4764,7 @@
         <v>81</v>
       </c>
       <c r="E33" t="s">
-        <v>122</v>
+        <v>26</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -4802,7 +4811,7 @@
         <v>82</v>
       </c>
       <c r="E34" t="s">
-        <v>122</v>
+        <v>26</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -4849,7 +4858,7 @@
         <v>83</v>
       </c>
       <c r="E35" t="s">
-        <v>124</v>
+        <v>26</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -4896,7 +4905,7 @@
         <v>84</v>
       </c>
       <c r="E36" t="s">
-        <v>123</v>
+        <v>26</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -4943,7 +4952,7 @@
         <v>80</v>
       </c>
       <c r="E37" t="s">
-        <v>122</v>
+        <v>26</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -4990,7 +4999,7 @@
         <v>81</v>
       </c>
       <c r="E38" t="s">
-        <v>122</v>
+        <v>26</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -5037,7 +5046,7 @@
         <v>85</v>
       </c>
       <c r="E39" t="s">
-        <v>122</v>
+        <v>26</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -5084,7 +5093,7 @@
         <v>83</v>
       </c>
       <c r="E40" t="s">
-        <v>124</v>
+        <v>26</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -5131,7 +5140,7 @@
         <v>86</v>
       </c>
       <c r="E41" t="s">
-        <v>123</v>
+        <v>26</v>
       </c>
       <c r="F41">
         <v>2</v>
@@ -5178,7 +5187,7 @@
         <v>87</v>
       </c>
       <c r="E42" t="s">
-        <v>122</v>
+        <v>25</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -5225,7 +5234,7 @@
         <v>80</v>
       </c>
       <c r="E43" t="s">
-        <v>122</v>
+        <v>25</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -5272,7 +5281,7 @@
         <v>85</v>
       </c>
       <c r="E44" t="s">
-        <v>122</v>
+        <v>25</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -5319,7 +5328,7 @@
         <v>83</v>
       </c>
       <c r="E45" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -5366,7 +5375,7 @@
         <v>81</v>
       </c>
       <c r="E46" t="s">
-        <v>123</v>
+        <v>25</v>
       </c>
       <c r="F46">
         <v>0</v>

</xml_diff>

<commit_message>
Updated rating system to be closer in spirit to SiegeGG's
</commit_message>
<xml_diff>
--- a/Output/Example.xlsx
+++ b/Output/Example.xlsx
@@ -23894,7 +23894,7 @@
         <v>65</v>
       </c>
       <c r="B2">
-        <v>0.8859008283479061</v>
+        <v>1.156316064300919</v>
       </c>
       <c r="C2">
         <v>82</v>
@@ -23959,7 +23959,7 @@
         <v>69</v>
       </c>
       <c r="B3">
-        <v>0.903413551338621</v>
+        <v>0.9859503970571286</v>
       </c>
       <c r="C3">
         <v>82</v>
@@ -24024,7 +24024,7 @@
         <v>68</v>
       </c>
       <c r="B4">
-        <v>0.8194107946906328</v>
+        <v>0.7446601105710036</v>
       </c>
       <c r="C4">
         <v>82</v>
@@ -24089,7 +24089,7 @@
         <v>66</v>
       </c>
       <c r="B5">
-        <v>0.8903843290652662</v>
+        <v>0.8363618024643859</v>
       </c>
       <c r="C5">
         <v>82</v>
@@ -24154,7 +24154,7 @@
         <v>67</v>
       </c>
       <c r="B6">
-        <v>0.8456908764426156</v>
+        <v>0.8248716278032237</v>
       </c>
       <c r="C6">
         <v>82</v>

</xml_diff>